<commit_message>
[FIX] Solved error in month data ranking table
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -994,10 +994,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4148"/>
+  <dimension ref="A1:C4150"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4123" workbookViewId="0">
-      <selection activeCell="D4142" sqref="D4142"/>
+    <sheetView tabSelected="1" topLeftCell="A4129" workbookViewId="0">
+      <selection activeCell="C4140" sqref="C4140:C4150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -46629,6 +46629,25 @@
         <v>10.4</v>
       </c>
     </row>
+    <row r="4149" spans="1:3">
+      <c r="A4149" s="1">
+        <v>4147</v>
+      </c>
+      <c r="B4149" s="2">
+        <v>45787</v>
+      </c>
+      <c r="C4149">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="4150" spans="1:2">
+      <c r="A4150" s="1">
+        <v>4148</v>
+      </c>
+      <c r="B4150" s="2">
+        <v>45788</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
[UPD] Updated database and indicators page
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="8280"/>
+    <workbookView windowWidth="23040" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Manual rain gage data" sheetId="1" r:id="rId1"/>
@@ -997,7 +997,7 @@
   <dimension ref="A1:C4231"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4209" workbookViewId="0">
-      <selection activeCell="C4213" sqref="C4213:C4219"/>
+      <selection activeCell="D4223" sqref="D4223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -47410,52 +47410,70 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4220" spans="1:2">
+    <row r="4220" spans="1:3">
       <c r="A4220" s="1">
         <v>4218</v>
       </c>
       <c r="B4220" s="2">
         <v>45858</v>
       </c>
-    </row>
-    <row r="4221" spans="1:2">
+      <c r="C4220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4221" spans="1:3">
       <c r="A4221" s="1">
         <v>4219</v>
       </c>
       <c r="B4221" s="2">
         <v>45859</v>
       </c>
-    </row>
-    <row r="4222" spans="1:2">
+      <c r="C4221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4222" spans="1:3">
       <c r="A4222" s="1">
         <v>4220</v>
       </c>
       <c r="B4222" s="2">
         <v>45860</v>
       </c>
-    </row>
-    <row r="4223" spans="1:2">
+      <c r="C4222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4223" spans="1:3">
       <c r="A4223" s="1">
         <v>4221</v>
       </c>
       <c r="B4223" s="2">
         <v>45861</v>
       </c>
-    </row>
-    <row r="4224" spans="1:2">
+      <c r="C4223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4224" spans="1:3">
       <c r="A4224" s="1">
         <v>4222</v>
       </c>
       <c r="B4224" s="2">
         <v>45862</v>
       </c>
-    </row>
-    <row r="4225" spans="1:2">
+      <c r="C4224">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4225" spans="1:3">
       <c r="A4225" s="1">
         <v>4223</v>
       </c>
       <c r="B4225" s="2">
         <v>45863</v>
+      </c>
+      <c r="C4225">
+        <v>4.2</v>
       </c>
     </row>
     <row r="4226" spans="1:2">

</xml_diff>

<commit_message>
[UPD] Updated database, added error plots and metrics for precipitation, and fixed indicators count warm nights in interactive plots
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -994,10 +994,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C4304"/>
+  <dimension ref="A1:C4310"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4284" workbookViewId="0">
-      <selection activeCell="C4305" sqref="C4305"/>
+    <sheetView tabSelected="1" topLeftCell="A4290" workbookViewId="0">
+      <selection activeCell="C4311" sqref="C4311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="2"/>
@@ -30709,7 +30709,7 @@
         <v>44339</v>
       </c>
       <c r="C2701">
-        <v>0</v>
+        <v>9.8</v>
       </c>
     </row>
     <row r="2702" spans="1:3">
@@ -30720,7 +30720,7 @@
         <v>44340</v>
       </c>
       <c r="C2702">
-        <v>29.4</v>
+        <v>19.6</v>
       </c>
     </row>
     <row r="2703" spans="1:3">
@@ -31974,7 +31974,7 @@
         <v>44454</v>
       </c>
       <c r="C2816">
-        <v>0</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="2817" spans="1:3">
@@ -31985,7 +31985,7 @@
         <v>44455</v>
       </c>
       <c r="C2817">
-        <v>8.6</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="2818" spans="1:3">
@@ -37606,7 +37606,7 @@
         <v>44966</v>
       </c>
       <c r="C3328">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3329" spans="1:3">
@@ -37617,7 +37617,7 @@
         <v>44967</v>
       </c>
       <c r="C3329">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3330" spans="1:3">
@@ -42479,7 +42479,7 @@
         <v>45409</v>
       </c>
       <c r="C3771">
-        <v>0</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="3772" spans="1:3">
@@ -44096,7 +44096,7 @@
         <v>45556</v>
       </c>
       <c r="C3918">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="3919" spans="1:3">
@@ -44107,7 +44107,7 @@
         <v>45557</v>
       </c>
       <c r="C3919">
-        <v>1.8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3920" spans="1:3">
@@ -44998,7 +44998,7 @@
         <v>45638</v>
       </c>
       <c r="C4000">
-        <v>0.2</v>
+        <v>7.2</v>
       </c>
     </row>
     <row r="4001" spans="1:3">
@@ -45009,7 +45009,7 @@
         <v>45639</v>
       </c>
       <c r="C4001">
-        <v>7.2</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4002" spans="1:3">
@@ -46637,7 +46637,7 @@
         <v>45787</v>
       </c>
       <c r="C4149">
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4150" spans="1:3">
@@ -46648,7 +46648,7 @@
         <v>45788</v>
       </c>
       <c r="C4150">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4151" spans="1:3">
@@ -48343,6 +48343,72 @@
       </c>
       <c r="C4304">
         <v>27</v>
+      </c>
+    </row>
+    <row r="4305" spans="1:3">
+      <c r="A4305" s="1">
+        <v>4303</v>
+      </c>
+      <c r="B4305" s="2">
+        <v>45943</v>
+      </c>
+      <c r="C4305">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="4306" spans="1:3">
+      <c r="A4306" s="1">
+        <v>4304</v>
+      </c>
+      <c r="B4306" s="2">
+        <v>45944</v>
+      </c>
+      <c r="C4306">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4307" spans="1:3">
+      <c r="A4307" s="1">
+        <v>4305</v>
+      </c>
+      <c r="B4307" s="2">
+        <v>45945</v>
+      </c>
+      <c r="C4307">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="4308" spans="1:3">
+      <c r="A4308" s="1">
+        <v>4306</v>
+      </c>
+      <c r="B4308" s="2">
+        <v>45946</v>
+      </c>
+      <c r="C4308">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4309" spans="1:3">
+      <c r="A4309" s="1">
+        <v>4307</v>
+      </c>
+      <c r="B4309" s="2">
+        <v>45947</v>
+      </c>
+      <c r="C4309">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4310" spans="1:3">
+      <c r="A4310" s="1">
+        <v>4308</v>
+      </c>
+      <c r="B4310" s="2">
+        <v>45948</v>
+      </c>
+      <c r="C4310">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPD] Updated database. Added code lines to prepare pcp data to correct
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -792,7 +792,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -822,7 +822,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1143,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4318"/>
+  <dimension ref="A1:E4324"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A4304" workbookViewId="0">
+      <selection activeCell="C4324" sqref="C4324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -8560,7 +8559,7 @@
       <c r="B665" s="10">
         <v>42303</v>
       </c>
-      <c r="C665" s="16">
+      <c r="C665" s="15">
         <v>1.2</v>
       </c>
       <c r="D665">
@@ -9466,7 +9465,7 @@
       <c r="B746" s="10">
         <v>42384</v>
       </c>
-      <c r="C746" s="16">
+      <c r="C746" s="15">
         <v>3.6</v>
       </c>
       <c r="D746">
@@ -49722,10 +49721,76 @@
         <v>45956</v>
       </c>
       <c r="C4318">
-        <v>16.4</v>
+        <v>18.8</v>
       </c>
       <c r="E4318">
         <v>1</v>
+      </c>
+    </row>
+    <row r="4319" spans="1:3">
+      <c r="A4319" s="7">
+        <v>4317</v>
+      </c>
+      <c r="B4319" s="10">
+        <v>45957</v>
+      </c>
+      <c r="C4319">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4320" spans="1:3">
+      <c r="A4320" s="7">
+        <v>4318</v>
+      </c>
+      <c r="B4320" s="10">
+        <v>45958</v>
+      </c>
+      <c r="C4320">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4321" spans="1:3">
+      <c r="A4321" s="7">
+        <v>4319</v>
+      </c>
+      <c r="B4321" s="10">
+        <v>45959</v>
+      </c>
+      <c r="C4321">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4322" spans="1:3">
+      <c r="A4322" s="7">
+        <v>4320</v>
+      </c>
+      <c r="B4322" s="10">
+        <v>45960</v>
+      </c>
+      <c r="C4322">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="4323" spans="1:3">
+      <c r="A4323" s="7">
+        <v>4321</v>
+      </c>
+      <c r="B4323" s="10">
+        <v>45961</v>
+      </c>
+      <c r="C4323">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4324" spans="1:3">
+      <c r="A4324" s="7">
+        <v>4322</v>
+      </c>
+      <c r="B4324" s="10">
+        <v>45962</v>
+      </c>
+      <c r="C4324">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPD] Corrected daily precipitation database and unify column name for this variable in all modules
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -1142,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4324"/>
+  <dimension ref="A1:E4331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4304" workbookViewId="0">
-      <selection activeCell="C4324" sqref="C4324"/>
+    <sheetView tabSelected="1" topLeftCell="A4311" workbookViewId="0">
+      <selection activeCell="C4331" sqref="C4331"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -49791,6 +49791,89 @@
       </c>
       <c r="C4324">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="4325" spans="1:3">
+      <c r="A4325" s="7">
+        <v>4323</v>
+      </c>
+      <c r="B4325" s="10">
+        <v>45963</v>
+      </c>
+      <c r="C4325">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4326" spans="1:3">
+      <c r="A4326" s="7">
+        <v>4324</v>
+      </c>
+      <c r="B4326" s="10">
+        <v>45964</v>
+      </c>
+      <c r="C4326">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4327" spans="1:3">
+      <c r="A4327" s="7">
+        <v>4325</v>
+      </c>
+      <c r="B4327" s="10">
+        <v>45965</v>
+      </c>
+      <c r="C4327">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4328" spans="1:3">
+      <c r="A4328" s="7">
+        <v>4326</v>
+      </c>
+      <c r="B4328" s="10">
+        <v>45966</v>
+      </c>
+      <c r="C4328">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4329" spans="1:5">
+      <c r="A4329" s="7">
+        <v>4327</v>
+      </c>
+      <c r="B4329" s="10">
+        <v>45967</v>
+      </c>
+      <c r="C4329">
+        <v>37</v>
+      </c>
+      <c r="D4329">
+        <v>1</v>
+      </c>
+      <c r="E4329">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4330" spans="1:3">
+      <c r="A4330" s="7">
+        <v>4328</v>
+      </c>
+      <c r="B4330" s="10">
+        <v>45968</v>
+      </c>
+      <c r="C4330">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4331" spans="1:3">
+      <c r="A4331" s="7">
+        <v>4329</v>
+      </c>
+      <c r="B4331" s="10">
+        <v>45969</v>
+      </c>
+      <c r="C4331">
+        <v>30.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPD] Updated corrected database
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -1142,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4340"/>
+  <dimension ref="A1:E4344"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4317" workbookViewId="0">
-      <selection activeCell="E4340" sqref="E4340"/>
+    <sheetView tabSelected="1" topLeftCell="A4320" workbookViewId="0">
+      <selection activeCell="C4324" sqref="C4324:C4344"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -49984,6 +49984,62 @@
         <v>11</v>
       </c>
       <c r="E4340">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4341" spans="1:4">
+      <c r="A4341" s="7">
+        <v>4339</v>
+      </c>
+      <c r="B4341" s="10">
+        <v>45979</v>
+      </c>
+      <c r="C4341">
+        <v>1</v>
+      </c>
+      <c r="D4341">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4342" spans="1:3">
+      <c r="A4342" s="7">
+        <v>4340</v>
+      </c>
+      <c r="B4342" s="10">
+        <v>45980</v>
+      </c>
+      <c r="C4342">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4343" spans="1:4">
+      <c r="A4343" s="7">
+        <v>4341</v>
+      </c>
+      <c r="B4343" s="10">
+        <v>45981</v>
+      </c>
+      <c r="C4343">
+        <v>1.4</v>
+      </c>
+      <c r="D4343">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4344" spans="1:5">
+      <c r="A4344" s="7">
+        <v>4342</v>
+      </c>
+      <c r="B4344" s="10">
+        <v>45982</v>
+      </c>
+      <c r="C4344">
+        <v>3.8</v>
+      </c>
+      <c r="D4344">
+        <v>1</v>
+      </c>
+      <c r="E4344">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[UPD] Updated database and corrected daily rain
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -1142,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4344"/>
+  <dimension ref="A1:E4350"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4320" workbookViewId="0">
-      <selection activeCell="C4324" sqref="C4324:C4344"/>
+    <sheetView tabSelected="1" topLeftCell="A4324" workbookViewId="0">
+      <selection activeCell="C4324" sqref="C4324:C4350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -50040,6 +50040,84 @@
         <v>1</v>
       </c>
       <c r="E4344">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4345" spans="1:3">
+      <c r="A4345" s="7">
+        <v>4343</v>
+      </c>
+      <c r="B4345" s="10">
+        <v>45983</v>
+      </c>
+      <c r="C4345">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4346" spans="1:3">
+      <c r="A4346" s="7">
+        <v>4344</v>
+      </c>
+      <c r="B4346" s="10">
+        <v>45984</v>
+      </c>
+      <c r="C4346">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4347" spans="1:3">
+      <c r="A4347" s="7">
+        <v>4345</v>
+      </c>
+      <c r="B4347" s="10">
+        <v>45985</v>
+      </c>
+      <c r="C4347">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4348" spans="1:4">
+      <c r="A4348" s="7">
+        <v>4346</v>
+      </c>
+      <c r="B4348" s="10">
+        <v>45986</v>
+      </c>
+      <c r="C4348">
+        <v>1.4</v>
+      </c>
+      <c r="D4348">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4349" spans="1:5">
+      <c r="A4349" s="7">
+        <v>4347</v>
+      </c>
+      <c r="B4349" s="10">
+        <v>45987</v>
+      </c>
+      <c r="C4349">
+        <v>3.4</v>
+      </c>
+      <c r="D4349">
+        <v>1</v>
+      </c>
+      <c r="E4349">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4350" spans="1:4">
+      <c r="A4350" s="7">
+        <v>4348</v>
+      </c>
+      <c r="B4350" s="10">
+        <v>45988</v>
+      </c>
+      <c r="C4350">
+        <v>0.4</v>
+      </c>
+      <c r="D4350">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[UPD] Updated database, changed time baseline in cumulative plots
</commit_message>
<xml_diff>
--- a/data/daily_manual_rain_gage_data.xlsx
+++ b/data/daily_manual_rain_gage_data.xlsx
@@ -1142,10 +1142,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4373"/>
+  <dimension ref="A1:E4377"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4352" workbookViewId="0">
-      <selection activeCell="D4372" sqref="D4372"/>
+    <sheetView tabSelected="1" topLeftCell="A4357" workbookViewId="0">
+      <selection activeCell="D4375" sqref="D4375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4" outlineLevelCol="4"/>
@@ -50399,12 +50399,59 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4373" spans="1:2">
+    <row r="4373" spans="1:3">
       <c r="A4373" s="7">
         <v>4371</v>
       </c>
       <c r="B4373" s="10">
         <v>46011</v>
+      </c>
+      <c r="C4373">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="4374" spans="1:3">
+      <c r="A4374" s="7">
+        <v>4372</v>
+      </c>
+      <c r="B4374" s="10">
+        <v>46012</v>
+      </c>
+      <c r="C4374">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:3">
+      <c r="A4375" s="7">
+        <v>4373</v>
+      </c>
+      <c r="B4375" s="10">
+        <v>46013</v>
+      </c>
+      <c r="C4375">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:4">
+      <c r="A4376" s="7">
+        <v>4374</v>
+      </c>
+      <c r="B4376" s="10">
+        <v>46014</v>
+      </c>
+      <c r="C4376">
+        <v>12.8</v>
+      </c>
+      <c r="D4376">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:2">
+      <c r="A4377" s="7">
+        <v>4375</v>
+      </c>
+      <c r="B4377" s="10">
+        <v>46015</v>
       </c>
     </row>
   </sheetData>

</xml_diff>